<commit_message>
7.20 Done Personal Document.
</commit_message>
<xml_diff>
--- a/Personal Document/ChangJiaQi/个人日报 常家奇.xlsx
+++ b/Personal Document/ChangJiaQi/个人日报 常家奇.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="文件封面" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="62">
   <si>
     <t xml:space="preserve">密级：秘密</t>
   </si>
@@ -608,6 +608,38 @@
       <t xml:space="preserve">语言基础</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Droid Sans Fallback"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">基础</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">LinkedList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">内存和文件</t>
+  </si>
 </sst>
 </file>
 
@@ -617,7 +649,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="55">
+  <fonts count="56">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -968,6 +1000,11 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="Droid Sans Fallback"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1215,7 +1252,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1688,6 +1725,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1719,9 +1760,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>578160</xdr:colOff>
+      <xdr:colOff>577440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>230760</xdr:rowOff>
+      <xdr:rowOff>230040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1731,7 +1772,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5280480" y="233640"/>
-          <a:ext cx="340200" cy="279000"/>
+          <a:ext cx="339480" cy="278280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -1802,9 +1843,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>29520</xdr:colOff>
+      <xdr:colOff>28800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>235440</xdr:rowOff>
+      <xdr:rowOff>234720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1814,7 +1855,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5647320" y="296280"/>
-          <a:ext cx="299520" cy="221040"/>
+          <a:ext cx="298800" cy="220320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2858,9 +2899,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>336240</xdr:colOff>
+      <xdr:colOff>335520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>235800</xdr:rowOff>
+      <xdr:rowOff>235080</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2870,7 +2911,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5970600" y="301680"/>
-          <a:ext cx="282960" cy="216000"/>
+          <a:ext cx="282240" cy="215280"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3289,9 +3330,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>627120</xdr:colOff>
+      <xdr:colOff>626400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>235440</xdr:rowOff>
+      <xdr:rowOff>234720</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -3301,7 +3342,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6279840" y="296280"/>
-          <a:ext cx="264600" cy="221040"/>
+          <a:ext cx="263880" cy="220320"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -4470,9 +4511,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>80640</xdr:colOff>
+      <xdr:colOff>79920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>236880</xdr:rowOff>
+      <xdr:rowOff>236160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4482,7 +4523,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6563160" y="296280"/>
-          <a:ext cx="309960" cy="222480"/>
+          <a:ext cx="309240" cy="221760"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -5679,9 +5720,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>504000</xdr:colOff>
+      <xdr:colOff>503280</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>234720</xdr:rowOff>
+      <xdr:rowOff>234000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5691,7 +5732,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6887160" y="219240"/>
-          <a:ext cx="409320" cy="297360"/>
+          <a:ext cx="408600" cy="296640"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6352,9 +6393,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6368,7 +6409,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6394,9 +6435,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6410,7 +6451,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6436,9 +6477,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6452,7 +6493,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6478,9 +6519,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>359640</xdr:colOff>
+      <xdr:colOff>358920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>277920</xdr:rowOff>
+      <xdr:rowOff>277200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6490,7 +6531,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5940000" y="281520"/>
-          <a:ext cx="331200" cy="285840"/>
+          <a:ext cx="330480" cy="285120"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -6561,9 +6602,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>677520</xdr:colOff>
+      <xdr:colOff>676800</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>283320</xdr:rowOff>
+      <xdr:rowOff>282600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -6573,7 +6614,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6297120" y="345960"/>
-          <a:ext cx="291960" cy="226800"/>
+          <a:ext cx="291240" cy="226080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -7617,9 +7658,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>976320</xdr:colOff>
+      <xdr:colOff>975600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>283320</xdr:rowOff>
+      <xdr:rowOff>282600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -7629,7 +7670,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6612120" y="351360"/>
-          <a:ext cx="275760" cy="221400"/>
+          <a:ext cx="275040" cy="220680"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -8048,9 +8089,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1259640</xdr:colOff>
+      <xdr:colOff>1258920</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>283320</xdr:rowOff>
+      <xdr:rowOff>282600</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -8060,7 +8101,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6913440" y="345960"/>
-          <a:ext cx="257760" cy="226800"/>
+          <a:ext cx="257040" cy="226080"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -9229,9 +9270,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>72720</xdr:colOff>
+      <xdr:colOff>72000</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>284760</xdr:rowOff>
+      <xdr:rowOff>284040</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -9241,7 +9282,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7189200" y="345960"/>
-          <a:ext cx="302040" cy="228240"/>
+          <a:ext cx="301320" cy="227520"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -10438,9 +10479,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>484920</xdr:colOff>
+      <xdr:colOff>484200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>281880</xdr:rowOff>
+      <xdr:rowOff>281160</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -10450,7 +10491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7504920" y="266760"/>
-          <a:ext cx="398520" cy="304560"/>
+          <a:ext cx="397800" cy="303840"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -11111,9 +11152,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11127,7 +11168,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11153,9 +11194,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11169,7 +11210,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11195,9 +11236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11211,7 +11252,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11237,9 +11278,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11253,7 +11294,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11279,9 +11320,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11295,7 +11336,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11321,9 +11362,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11337,7 +11378,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -11363,9 +11404,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>541800</xdr:colOff>
+      <xdr:colOff>541080</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>523080</xdr:rowOff>
+      <xdr:rowOff>522360</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -11379,7 +11420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="10317960" y="76320"/>
-          <a:ext cx="2181240" cy="446760"/>
+          <a:ext cx="2180520" cy="446040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -14453,7 +14494,7 @@
   </sheetPr>
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -14890,8 +14931,8 @@
   </sheetPr>
   <dimension ref="B1:J27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E33" activeCellId="0" sqref="E33"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K16" activeCellId="0" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14937,19 +14978,27 @@
       <c r="B3" s="71" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="72"/>
+      <c r="C3" s="72" t="s">
+        <v>28</v>
+      </c>
       <c r="D3" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="73"/>
+      <c r="E3" s="73" t="n">
+        <v>720</v>
+      </c>
       <c r="F3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="74"/>
+      <c r="G3" s="74" t="s">
+        <v>54</v>
+      </c>
       <c r="H3" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="76"/>
+      <c r="I3" s="76" t="n">
+        <v>5</v>
+      </c>
       <c r="J3" s="74"/>
     </row>
     <row r="4" s="77" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14969,7 +15018,9 @@
       <c r="B5" s="82" t="s">
         <v>34</v>
       </c>
-      <c r="C5" s="83"/>
+      <c r="C5" s="83" t="s">
+        <v>57</v>
+      </c>
       <c r="D5" s="83"/>
       <c r="E5" s="83"/>
       <c r="F5" s="83"/>
@@ -14982,7 +15033,9 @@
       <c r="B6" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="85"/>
+      <c r="C6" s="85" t="n">
+        <v>720</v>
+      </c>
       <c r="D6" s="85"/>
       <c r="E6" s="85"/>
       <c r="F6" s="85"/>
@@ -14995,7 +15048,9 @@
       <c r="B7" s="86" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="87"/>
+      <c r="C7" s="87" t="n">
+        <v>720</v>
+      </c>
       <c r="D7" s="87"/>
       <c r="E7" s="87"/>
       <c r="F7" s="87"/>
@@ -15042,27 +15097,43 @@
       <c r="B10" s="97" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="98"/>
+      <c r="C10" s="98" t="s">
+        <v>58</v>
+      </c>
       <c r="D10" s="98"/>
       <c r="E10" s="98"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="100"/>
+      <c r="F10" s="99" t="n">
+        <v>5</v>
+      </c>
+      <c r="G10" s="100" t="s">
+        <v>59</v>
+      </c>
       <c r="H10" s="100"/>
       <c r="I10" s="100"/>
-      <c r="J10" s="101"/>
+      <c r="J10" s="101" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" s="96" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="97" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="98"/>
-      <c r="D11" s="98"/>
-      <c r="E11" s="98"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="100"/>
+      <c r="C11" s="118" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="118"/>
+      <c r="E11" s="118"/>
+      <c r="F11" s="99" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" s="100" t="s">
+        <v>59</v>
+      </c>
       <c r="H11" s="100"/>
       <c r="I11" s="100"/>
-      <c r="J11" s="101"/>
+      <c r="J11" s="101" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" s="96" customFormat="true" ht="20.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="102" t="n">
@@ -15138,7 +15209,7 @@
       <c r="E17" s="103"/>
       <c r="F17" s="104" t="n">
         <f aca="false">SUM(F10:F16)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="G17" s="105"/>
       <c r="H17" s="105"/>
@@ -15179,9 +15250,13 @@
       <c r="B20" s="109" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="110"/>
+      <c r="C20" s="110" t="s">
+        <v>51</v>
+      </c>
       <c r="D20" s="110"/>
-      <c r="E20" s="111"/>
+      <c r="E20" s="111" t="s">
+        <v>51</v>
+      </c>
       <c r="F20" s="111"/>
       <c r="G20" s="111"/>
       <c r="H20" s="111"/>

</xml_diff>